<commit_message>
refactor: Improve Kyorugi tab UI and options
</commit_message>
<xml_diff>
--- a/templates/겨루기_경기시간_계산기_양식.xlsx
+++ b/templates/겨루기_경기시간_계산기_양식.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,76 +424,20 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>종목</t>
+          <t>참가부</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>참가부</t>
+          <t>체급</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
-        <is>
-          <t>세부부별</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>성별</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
         <is>
           <t>인원수</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>겨루기</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>초등부</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>-40kg</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>남자</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>겨루기</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>중등부</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>-50kg</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>여자</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>